<commit_message>
Work Log -- Michael Beaver
Updated work log for Michael Beaver.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Developed template for log of hours worked for each team member. Recored own work hours.</t>
+  </si>
+  <si>
+    <t>Purchased 3" three-ring binder and two packs of 8-tab separators.</t>
+  </si>
+  <si>
+    <t>Team meeting. Recorded meeting minutes. Began high-level design of backend and described high-level frontend features.</t>
   </si>
 </sst>
 </file>
@@ -345,12 +351,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,11 +359,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -373,70 +436,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -742,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:H10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -757,13 +763,13 @@
   <sheetData>
     <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -771,127 +777,127 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="6" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
+      <c r="A5" s="13">
         <v>41653</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
         <v>41660</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="14">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+      <c r="A7" s="16">
         <v>41660</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="20">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="12">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="A8" s="16">
         <v>41662</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="20">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="A9" s="16">
+        <v>41665</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
         <v>41666</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="20">
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
         <v>41667</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B11" s="23" t="s">
         <v>6</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="20">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
-        <v>41667</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>10</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -899,411 +905,421 @@
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="20">
-        <v>1.17</v>
+      <c r="I11" s="12">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="16">
+        <v>41667</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="20"/>
+      <c r="I12" s="12">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="20"/>
+      <c r="A13" s="16">
+        <v>41670</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="12">
+        <v>3.75</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="20"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="20"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="20"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="20"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="20"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="20"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="20"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="20"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="20"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="20"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="37"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="35"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="6" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="37"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="20"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="20"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="20"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="20"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="20"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="20"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="20"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="20"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="20"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="20"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="20"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="20"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="20"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="20"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="20"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="20"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="20"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="I45" s="8"/>
+      <c r="A45" s="5"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="17">
+      <c r="G46" s="36"/>
+      <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="I46" s="17"/>
+        <v>13.95</v>
+      </c>
+      <c r="I46" s="37"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
       <c r="I47" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="H46:I46"/>
@@ -1313,36 +1329,38 @@
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B17:H17"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B11:H11"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documents -- Updated Work Log
This is the work log for Michael updated to include independent work on
initial tentative prototype.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Team meeting. Recorded meeting minutes. Began high-level design of backend and described high-level frontend features.</t>
+  </si>
+  <si>
+    <t>Created initial tentative prototype with extremely limited functionality (mostly message boxes).</t>
   </si>
 </sst>
 </file>
@@ -397,36 +400,45 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -435,15 +447,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +752,7 @@
   <dimension ref="A2:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B14" sqref="B14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -763,13 +766,13 @@
   <sheetData>
     <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -777,15 +780,15 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
       <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
@@ -794,15 +797,15 @@
       <c r="A5" s="13">
         <v>41653</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="10">
         <v>2</v>
       </c>
@@ -811,15 +814,15 @@
       <c r="A6" s="17">
         <v>41660</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="14">
         <v>1.5</v>
       </c>
@@ -828,15 +831,15 @@
       <c r="A7" s="16">
         <v>41660</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="12">
         <v>0.6</v>
       </c>
@@ -845,15 +848,15 @@
       <c r="A8" s="16">
         <v>41662</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="12">
         <v>1</v>
       </c>
@@ -862,15 +865,15 @@
       <c r="A9" s="16">
         <v>41665</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="12">
         <v>0.25</v>
       </c>
@@ -879,15 +882,15 @@
       <c r="A10" s="16">
         <v>41666</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="12">
         <v>2.5</v>
       </c>
@@ -896,15 +899,15 @@
       <c r="A11" s="16">
         <v>41667</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -913,15 +916,15 @@
       <c r="A12" s="16">
         <v>41667</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
       <c r="I12" s="12">
         <v>1.25</v>
       </c>
@@ -930,364 +933,370 @@
       <c r="A13" s="16">
         <v>41670</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="12">
         <v>3.75</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="16">
+        <v>41670</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
       <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
       <c r="I26" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24"/>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="28"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="28"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="28"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24"/>
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="28"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="24"/>
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="28"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="24"/>
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="28"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="24"/>
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="24"/>
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="27"/>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1300,15 +1309,15 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37">
+      <c r="G46" s="28"/>
+      <c r="H46" s="29">
         <f>SUM(I5:I44)</f>
-        <v>13.95</v>
-      </c>
-      <c r="I46" s="37"/>
+        <v>15.95</v>
+      </c>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F47" s="7"/>
@@ -1317,6 +1326,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B27:H27"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B43:H43"/>
     <mergeCell ref="B22:H22"/>
@@ -1333,34 +1370,6 @@
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documents -- Minutes, Questions, Work Log
This update contains the Feb. 23 meeting minutes, client questions #3,
and my work log.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Created initial tentative prototype with extremely limited functionality (mostly message boxes).</t>
+  </si>
+  <si>
+    <t>Team meeting. Recorded meeting minutes. Worked on refining tentative prototype model for client critique at the next client meeting.</t>
   </si>
 </sst>
 </file>
@@ -400,6 +403,18 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -409,13 +424,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -423,30 +450,6 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,7 +755,7 @@
   <dimension ref="A2:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:H14"/>
+      <selection activeCell="B16" sqref="B16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -766,13 +769,13 @@
   <sheetData>
     <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -780,15 +783,15 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
       <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
@@ -797,15 +800,15 @@
       <c r="A5" s="13">
         <v>41653</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="10">
         <v>2</v>
       </c>
@@ -814,15 +817,15 @@
       <c r="A6" s="17">
         <v>41660</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="14">
         <v>1.5</v>
       </c>
@@ -831,15 +834,15 @@
       <c r="A7" s="16">
         <v>41660</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="12">
         <v>0.6</v>
       </c>
@@ -848,15 +851,15 @@
       <c r="A8" s="16">
         <v>41662</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="12">
         <v>1</v>
       </c>
@@ -865,15 +868,15 @@
       <c r="A9" s="16">
         <v>41665</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="12">
         <v>0.25</v>
       </c>
@@ -882,15 +885,15 @@
       <c r="A10" s="16">
         <v>41666</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="12">
         <v>2.5</v>
       </c>
@@ -899,15 +902,15 @@
       <c r="A11" s="16">
         <v>41667</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -916,15 +919,15 @@
       <c r="A12" s="16">
         <v>41667</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="12">
         <v>1.25</v>
       </c>
@@ -933,15 +936,15 @@
       <c r="A13" s="16">
         <v>41670</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
       <c r="I13" s="12">
         <v>3.75</v>
       </c>
@@ -950,353 +953,359 @@
       <c r="A14" s="16">
         <v>41670</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="16">
+        <v>41674</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="12">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="24"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="24"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="28"/>
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="24"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="28"/>
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
       <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="24"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="28"/>
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="24"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="28"/>
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="24"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="28"/>
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="24"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="28"/>
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="24"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="28"/>
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="24"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="28"/>
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="27"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="25"/>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,15 +1318,15 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F46" s="28" t="s">
+      <c r="F46" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="28"/>
-      <c r="H46" s="29">
+      <c r="G46" s="36"/>
+      <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>15.95</v>
-      </c>
-      <c r="I46" s="29"/>
+        <v>18.2</v>
+      </c>
+      <c r="I46" s="37"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F47" s="7"/>
@@ -1326,6 +1335,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B27:H27"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B9:H9"/>
@@ -1342,34 +1379,6 @@
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documents -- Minutes, Client Questions, Work Log
This update contains the minutes for the Feb. 4 client meeting. The CASE
Tools list has been updated, as well.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Team meeting. Recorded meeting minutes. Worked on refining tentative prototype model for client critique at the next client meeting.</t>
+  </si>
+  <si>
+    <t>Modified and updated prototype for client meeting.</t>
   </si>
 </sst>
 </file>
@@ -754,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:H16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -968,7 +971,7 @@
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
-        <v>41674</v>
+        <v>41673</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>14</v>
@@ -984,26 +987,38 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="16">
+        <v>41674</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="12"/>
+      <c r="A17" s="16">
+        <v>41674</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="12">
+        <v>2.15</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
@@ -1324,7 +1339,7 @@
       <c r="G46" s="36"/>
       <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>18.2</v>
+        <v>21.349999999999998</v>
       </c>
       <c r="I46" s="37"/>
     </row>

</xml_diff>

<commit_message>
Documents -- Work Log
Updated work log.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Modified and updated prototype for client meeting.</t>
+  </si>
+  <si>
+    <t>Created initial draft of specifications document. Began drafting the introductory sections.</t>
+  </si>
+  <si>
+    <t>Read IEEE Standard 830-1998 recommendations for specifications documents. Updated specifications document to version 1.0.1 to include definitions, acronyms, abbreviations, update procedures, and appendices.</t>
+  </si>
+  <si>
+    <t>Impromptu team meeting. Recorded meeting minutes. Set times for next two team meetings.</t>
   </si>
 </sst>
 </file>
@@ -757,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1021,37 +1030,55 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="16">
+        <v>41675</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>16</v>
+      </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="26"/>
+      <c r="I18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="16">
+        <v>41676</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>17</v>
+      </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
       <c r="H19" s="28"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="12">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="16">
+        <v>41676</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>18</v>
+      </c>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="27"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="12">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
@@ -1339,7 +1366,7 @@
       <c r="G46" s="36"/>
       <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>21.349999999999998</v>
+        <v>26.099999999999998</v>
       </c>
       <c r="I46" s="37"/>
     </row>

</xml_diff>

<commit_message>
Documents -- Minutes, SRS, Work Log, CASE Tools
This update contains Feb. 7 and Feb. 8 meeting minutes, SRS revisions, a
work log, and CASE tools list.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>Impromptu team meeting. Recorded meeting minutes. Set times for next two team meetings.</t>
+  </si>
+  <si>
+    <t>Team meeting. Recorded meeting minutes. Continued drafting software requirements specification document. Discussed high-level design problems and solutions. Developed additional client questions.</t>
+  </si>
+  <si>
+    <t>Heavily updated software requirements specification document by adding sections and updating information.</t>
+  </si>
+  <si>
+    <t>Team meeting. Recorded meeting minutes. Continued drafting software requirements specification document. Contributed to prototype user interface color scheme discussions.</t>
+  </si>
+  <si>
+    <t>Completed the first major draft revision of the software requirements specification document.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -462,6 +474,9 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:H23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -856,7 +871,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
       <c r="I7" s="12">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,48 +1096,72 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="16">
+        <v>41677</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="16">
+        <v>41677</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="16">
+        <v>41678</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="38">
+        <v>41678</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="21"/>
+      <c r="I24" s="21">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
@@ -1366,7 +1405,7 @@
       <c r="G46" s="36"/>
       <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>26.099999999999998</v>
+        <v>36.75</v>
       </c>
       <c r="I46" s="37"/>
     </row>

</xml_diff>

<commit_message>
Documents -- Questions, Proposal, Minutes, Log
This update contains client questions #4, programming language proposal,
meeting minutes, and my work log.
</commit_message>
<xml_diff>
--- a/Documents/Work Logs/Michael Beaver.xlsx
+++ b/Documents/Work Logs/Michael Beaver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Completed the first major draft revision of the software requirements specification document.</t>
+  </si>
+  <si>
+    <t>Updated the software requirements specification document as per Travis's comments and suggestions. Drafted programming language proposal.</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -421,12 +424,12 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -474,9 +477,6 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:H24"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1147,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="38">
+      <c r="A24" s="21">
         <v>41678</v>
       </c>
       <c r="B24" s="23" t="s">
@@ -1159,7 +1159,7 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="21">
+      <c r="I24" s="20">
         <v>1.25</v>
       </c>
     </row>
@@ -1192,26 +1192,38 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="21">
+        <v>41683</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>23</v>
+      </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="21"/>
+      <c r="I27" s="20">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="12"/>
+      <c r="A28" s="16">
+        <v>41683</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="12">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
@@ -1405,7 +1417,7 @@
       <c r="G46" s="36"/>
       <c r="H46" s="37">
         <f>SUM(I5:I44)</f>
-        <v>36.75</v>
+        <v>38.75</v>
       </c>
       <c r="I46" s="37"/>
     </row>

</xml_diff>